<commit_message>
rerun code after translation updates
</commit_message>
<xml_diff>
--- a/data/relevant frame selection/authority_frames.xlsx
+++ b/data/relevant frame selection/authority_frames.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="205">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -61,6 +61,21 @@
     <t>arresteren</t>
   </si>
   <si>
+    <t>depecheren</t>
+  </si>
+  <si>
+    <t>onderteekent</t>
+  </si>
+  <si>
+    <t>remitteren</t>
+  </si>
+  <si>
+    <t>belegeren</t>
+  </si>
+  <si>
+    <t>veroveren</t>
+  </si>
+  <si>
     <t>handhaven</t>
   </si>
   <si>
@@ -100,9 +115,15 @@
     <t>inwilligen</t>
   </si>
   <si>
+    <t>nacomen</t>
+  </si>
+  <si>
     <t>remitteeren</t>
   </si>
   <si>
+    <t>toegestaen</t>
+  </si>
+  <si>
     <t>twisten</t>
   </si>
   <si>
@@ -130,6 +151,21 @@
     <t>arresteren:14</t>
   </si>
   <si>
+    <t>depecheren:9</t>
+  </si>
+  <si>
+    <t>onderteekent:9</t>
+  </si>
+  <si>
+    <t>remitteren:9</t>
+  </si>
+  <si>
+    <t>belegeren:8</t>
+  </si>
+  <si>
+    <t>veroveren:8</t>
+  </si>
+  <si>
     <t>handhaven:6</t>
   </si>
   <si>
@@ -169,9 +205,15 @@
     <t>inwilligen:5</t>
   </si>
   <si>
+    <t>nacomen:5</t>
+  </si>
+  <si>
     <t>remitteeren:5</t>
   </si>
   <si>
+    <t>toegestaen:5</t>
+  </si>
+  <si>
     <t>twisten:5</t>
   </si>
   <si>
@@ -199,6 +241,21 @@
     <t>{M004402:arresteren:VRB}</t>
   </si>
   <si>
+    <t>{A004124:depêcheren:VRB}</t>
+  </si>
+  <si>
+    <t>{M043720:ondertekenen:VRB,34855:ondertekenen:VRB}</t>
+  </si>
+  <si>
+    <t>{M058787:remitteren:VRB}</t>
+  </si>
+  <si>
+    <t>{M006773:belegeren:VRB}</t>
+  </si>
+  <si>
+    <t>{M077424:veroveren:VRB}</t>
+  </si>
+  <si>
     <t>{M023804:handhaven:VRB,"M023803:handhaaf, handhave:NOU-C"}</t>
   </si>
   <si>
@@ -238,7 +295,10 @@
     <t>{M028373:inwilligen:VRB}</t>
   </si>
   <si>
-    <t>{M058787:remitteren:VRB}</t>
+    <t>{31722:nakomen:VRB}</t>
+  </si>
+  <si>
+    <t>{58608:toestaan:VRB,M068927:toestaan:VRB}</t>
   </si>
   <si>
     <t>{60081:twisten:VRB,M071555:twisten:VRB,M071551.re.1:twisten:,60076:twist:NOU-C,M071550:twist:NOU-C,A015067.re.1:twisten:,GH20191029.115756.199:twisten:VRB,M071551:twist:NOU-C}</t>
@@ -253,18 +313,30 @@
     <t>{M080118:vigileren:VRB}</t>
   </si>
   <si>
+    <t>sturen; zenden</t>
+  </si>
+  <si>
+    <t>achtervolgen; achternagaan; in de buurt komen; dichtbij komen</t>
+  </si>
+  <si>
     <t xml:space="preserve">verschaffen; leveren; afleveren </t>
   </si>
   <si>
     <t>overhandigen; overleveren; overdragen</t>
   </si>
   <si>
-    <t>regelen; ordenen; inrichten</t>
+    <t>regelen; ordenen; inrichten; schikken</t>
   </si>
   <si>
     <t>arresteren; beslag leggen op; besluiten; vaststellen</t>
   </si>
   <si>
+    <t>ondertekenen; tekenen</t>
+  </si>
+  <si>
+    <t>vergeven; kwijtschelden</t>
+  </si>
+  <si>
     <t>vasthouden; beheren; in beslag nemen; aanhouden</t>
   </si>
   <si>
@@ -295,148 +367,184 @@
     <t>inwilligen, toestaan</t>
   </si>
   <si>
-    <t>vergeven; kwijtschelden</t>
+    <t>opvolgen</t>
+  </si>
+  <si>
+    <t>toestaan</t>
   </si>
   <si>
     <t>twisten; het oneens zijn; ruzie maken; strijden; strijd voeren</t>
   </si>
   <si>
-    <t>gebieden; verkondigen; bekendmaken</t>
+    <t>gebieden; verkondigen; bekendmaken; verbieden</t>
   </si>
   <si>
     <t>waken over; waakzaam zijn; bewaken; toezicht houden op</t>
   </si>
   <si>
-    <t>['Bringing', 'Submitting_documents', 'Surrendering', 'Giving', 'Transfer', 'Causation']</t>
-  </si>
-  <si>
-    <t>['Judgment', 'Successful_action', 'Bail_setting', 'Removing', 'Success_or_failure']</t>
-  </si>
-  <si>
-    <t>['Activity_stop', 'Deciding', 'Cause_to_end', 'Choosing', 'Activity_finish', 'Kidnapping', 'Firing', 'Arrest', 'Coming_to_believe', 'Killing']</t>
-  </si>
-  <si>
-    <t>['Statement', 'Inhibit_movement', 'Hiring', 'Inchoative_attaching', 'Success_or_failure', 'Wearing', 'Kidnapping', 'Arrest', 'Manipulation', 'Successful_action', 'Activity_ongoing', 'Change_event_time', 'Detaining']</t>
-  </si>
-  <si>
-    <t>['Talking_into', 'Causation', 'Bringing', 'Removing', 'Experiencer_obj', 'Influence_of_event_on_cognizer', 'Cotheme', 'Taking', 'Leadership']</t>
-  </si>
-  <si>
-    <t>['Adopt_selection', 'Imposing_obligation', 'Attempt_suasion']</t>
-  </si>
-  <si>
-    <t>['Judgment', 'Commerce_collect', 'Gathering_up', 'Frugality', 'Come_together', 'Removing', 'Experiencer_focus']</t>
-  </si>
-  <si>
-    <t>['Quarreling', 'Hostile_encounter']</t>
-  </si>
-  <si>
-    <t>['Filling', 'Being_in_operation', 'Assistance', 'Ingest_substance', 'Ingestion', 'Operating_a_system', 'Using', 'Rite', 'Intentionally_affect']</t>
+    <t>['Surrendering', 'Giving', 'Transfer', 'Bringing', 'Submitting_documents', 'Causation']</t>
+  </si>
+  <si>
+    <t>['Adjusting', 'Compliance', 'Bail_setting', 'Successful_action', 'Success_or_failure', 'Judgment', 'Choosing', 'Removing']</t>
+  </si>
+  <si>
+    <t>['Kidnapping', 'Cause_to_end', 'Activity_stop', 'Deciding', 'Firing', 'Coming_to_believe', 'Activity_finish', 'Choosing', 'Arrest', 'Killing']</t>
+  </si>
+  <si>
+    <t>['Using', 'Operating_a_system', 'Sending', 'Being_in_operation', 'Influence_of_event_on_cognizer']</t>
+  </si>
+  <si>
+    <t>['Text_creation', 'Get_a_job']</t>
+  </si>
+  <si>
+    <t>['Giving', 'Dispersal']</t>
   </si>
   <si>
     <t>[]</t>
   </si>
   <si>
-    <t>['Talking_into', 'Sending', 'Causation', 'Bringing', 'Removing', 'Experiencer_obj', 'Contacting', 'Influence_of_event_on_cognizer', 'Cotheme', 'Taking', 'Leadership']</t>
+    <t>['Kidnapping', 'Inchoative_attaching', 'Successful_action', 'Inhibit_movement', 'Manipulation', 'Change_event_time', 'Success_or_failure', 'Hiring', 'Statement', 'Detaining', 'Wearing', 'Arrest', 'Activity_ongoing']</t>
+  </si>
+  <si>
+    <t>['Leadership', 'Taking', 'Talking_into', 'Bringing', 'Experiencer_obj', 'Cotheme', 'Causation', 'Removing', 'Influence_of_event_on_cognizer']</t>
+  </si>
+  <si>
+    <t>['Adopt_selection', 'Attempt_suasion', 'Imposing_obligation']</t>
+  </si>
+  <si>
+    <t>['Experiencer_focus', 'Judgment', 'Commerce_collect', 'Come_together', 'Frugality', 'Gathering_up', 'Removing']</t>
+  </si>
+  <si>
+    <t>['Hostile_encounter', 'Quarreling']</t>
+  </si>
+  <si>
+    <t>['Intentionally_affect', 'Using', 'Ingestion', 'Filling', 'Operating_a_system', 'Assistance', 'Ingest_substance', 'Being_in_operation', 'Rite']</t>
+  </si>
+  <si>
+    <t>['Leadership', 'Taking', 'Contacting', 'Talking_into', 'Bringing', 'Experiencer_obj', 'Cotheme', 'Sending', 'Causation', 'Removing', 'Influence_of_event_on_cognizer']</t>
   </si>
   <si>
     <t>['Reveal_secret', 'Statement']</t>
   </si>
   <si>
-    <t>['Judgment_communication', 'Sentencing']</t>
-  </si>
-  <si>
-    <t>['Dispersal', 'Giving']</t>
-  </si>
-  <si>
-    <t>['Jury_deliberation', 'Hostile_encounter', 'Quarreling', 'Discussion']</t>
-  </si>
-  <si>
-    <t>['Giving', 'Submitting_documents', 'Surrendering', 'Causation']</t>
-  </si>
-  <si>
-    <t>['Needing', 'Judgment_communication', 'Required_event', 'Taking_time', 'Imposing_obligation', 'Judgment', 'Have_as_requirement', 'Request', 'Omen', 'Leadership']</t>
-  </si>
-  <si>
-    <t>['Bringing', 'Giving', 'Intentionally_act', 'Transfer', 'Delivery', 'Desiring', 'Successfully_communicate_message', 'Cotheme', 'Motion']</t>
-  </si>
-  <si>
-    <t>['Supply', 'Working_on', 'Execution', 'Posing_as', 'Separating', 'Adjusting', 'Leadership', 'Work', 'Dressing', 'Placing', 'Verdict', 'Building', 'Successful_action', 'Success_or_failure', 'Categorization', 'Setting_out', 'Ingestion', 'Departing', 'Being_employed', 'Cooking_creation', 'Change_event_time', 'Cause_to_start', 'Imprisonment', 'Assistance', 'Change_of_consistency', 'Differentiation', 'Encoding', 'Feigning', 'Cause_change_of_consistency', 'Arranging', 'Causation']</t>
-  </si>
-  <si>
-    <t>['Working_on', 'Activity_stop', 'Deciding', 'Cause_to_end', 'Contingency', 'Reasoning', 'Process_end', 'Taking', 'Coming_to_believe', 'Work', 'Activity_finish', 'Firing', 'Being_employed', 'Change_of_leadership', 'Notification_of_charges', 'Choosing', 'Commerce_collect', 'Manipulation', 'Killing']</t>
-  </si>
-  <si>
-    <t>['Activity_stop', 'Being_in_operation', 'Inchoative_attaching', 'Becoming', 'Operating_a_system', 'Resolve_problem', 'Compliance', 'Process_continue', 'Taking', 'Leadership', 'Halt', 'Change_position_on_a_scale', 'Placing', 'Being_attached', 'Success_or_failure', 'Cause_motion', 'Motion', 'Retaining', 'Containing', 'Attaching', 'Cause_change_of_position_on_a_scale', 'Travel', 'Self_motion', 'Change_event_time', 'Defend', 'Manipulation', 'Change_event_duration', 'Process_stop', 'Using', 'Successful_action', 'Activity_ongoing']</t>
-  </si>
-  <si>
-    <t>['Being_in_operation', 'Cause_to_make_progress', 'Resolve_problem', 'Operating_a_system', 'Taking', 'Leadership', 'Bringing', 'Verdict', 'Removing', 'Success_or_failure', 'Causation', 'Influence_of_event_on_cognizer', 'Self_motion', 'Change_of_leadership', 'Cotheme', 'Intentionally_act', 'Intentionally_create', 'Using', 'Successful_action']</t>
-  </si>
-  <si>
-    <t>['Containing', 'Imposing_obligation', 'Attempt_suasion', 'Impact', 'Objective_influence', 'Adopt_selection', 'Manipulation', 'Cause_to_move_in_place', 'Change_of_leadership', 'Being_in_effect', 'Cause_motion']</t>
-  </si>
-  <si>
-    <t>['Execution', 'Posing_as', 'Judgment', 'Possession', 'Dressing', 'Placing', 'Building', 'Cause_motion', 'Setting_out', 'Ingestion', 'Departing', 'Cooking_creation', 'Change_event_time', 'Cause_to_start', 'Imprisonment', 'Experiencer_focus', 'Change_of_consistency', 'Encoding', 'Feigning', 'Cause_change_of_consistency', 'Causation']</t>
-  </si>
-  <si>
-    <t>['Work', 'Working_on', 'Giving', 'Assistance', 'Being_in_operation', 'Using_resource', 'Resolve_problem', 'Operating_a_system', 'Being_employed', 'Employing', 'Using', 'Successful_action', 'Intentionally_affect', 'Self_motion', 'Success_or_failure', 'Leadership']</t>
-  </si>
-  <si>
-    <t>['Avoiding', 'Communication_manner', 'Motion']</t>
-  </si>
-  <si>
-    <t>['Being_in_operation', 'Cause_to_make_progress', 'Resolve_problem', 'Operating_a_system', 'Taking', 'Leadership', 'Bringing', 'Verdict', 'Removing', 'Success_or_failure', 'Operate_vehicle', 'Cause_motion', 'Causation', 'Influence_of_event_on_cognizer', 'Self_motion', 'Change_of_leadership', 'Cotheme', 'Intentionally_act', 'Intentionally_create', 'Using', 'Successful_action']</t>
-  </si>
-  <si>
-    <t>['Awareness', 'Statement', 'Verification', 'Commitment', 'Receiving', 'Reveal_secret', 'Respond_to_proposal']</t>
-  </si>
-  <si>
-    <t>['Judgment_communication', 'Verdict', 'Cause_harm', 'Sentencing', 'Cause_motion']</t>
-  </si>
-  <si>
-    <t>['Departing', 'Quitting_a_place', 'Competition']</t>
-  </si>
-  <si>
-    <t>['Assistance', 'Supply', 'Forgiveness']</t>
-  </si>
-  <si>
-    <t>['Friction', 'Hostile_encounter', 'Undergo_change', 'Cause_to_move_in_place', 'Moving_in_place', 'Change_direction', 'Self_motion', 'Quarreling']</t>
-  </si>
-  <si>
-    <t>['Extradition', 'Motion', 'Giving']</t>
-  </si>
-  <si>
-    <t>['Telling', 'Reporting', 'Filling', 'Statement', 'Imposing_obligation', 'Dispersal', 'Verdict', 'Request', 'Speak_on_topic', 'Motion', 'Leadership']</t>
-  </si>
-  <si>
-    <t>{'Transfer', 'Bringing', 'Giving'}</t>
-  </si>
-  <si>
-    <t>{'Success_or_failure', 'Successful_action'}</t>
-  </si>
-  <si>
-    <t>{'Activity_stop', 'Deciding', 'Cause_to_end', 'Choosing', 'Activity_finish', 'Firing', 'Killing', 'Coming_to_believe'}</t>
-  </si>
-  <si>
-    <t>{'Inchoative_attaching', 'Activity_ongoing', 'Manipulation', 'Successful_action', 'Success_or_failure', 'Change_event_time'}</t>
-  </si>
-  <si>
-    <t>{'Bringing', 'Causation', 'Influence_of_event_on_cognizer', 'Removing', 'Cotheme', 'Taking', 'Leadership'}</t>
+    <t>['Sentencing', 'Judgment_communication']</t>
+  </si>
+  <si>
+    <t>['Relative_time', 'Success_or_failure', 'Successful_action']</t>
+  </si>
+  <si>
+    <t>['Grant_permission', 'Permitting']</t>
+  </si>
+  <si>
+    <t>['Hostile_encounter', 'Jury_deliberation', 'Discussion', 'Quarreling']</t>
+  </si>
+  <si>
+    <t>['Causation', 'Giving', 'Submitting_documents', 'Surrendering']</t>
+  </si>
+  <si>
+    <t>['Needing', 'Leadership', 'Imposing_obligation', 'Request', 'Have_as_requirement', 'Required_event', 'Judgment', 'Preventing', 'Taking_time', 'Judgment_communication', 'Omen', 'Prohibiting', 'Deny_permission']</t>
+  </si>
+  <si>
+    <t>['Motion', 'Giving', 'Transfer', 'Bringing', 'Delivery', 'Cotheme', 'Intentionally_act', 'Desiring', 'Successfully_communicate_message']</t>
+  </si>
+  <si>
+    <t>['Adjusting', 'Imprisonment', 'Departing', 'Ingestion', 'Assistance', 'Being_employed', 'Encoding', 'Separating', 'Choosing', 'Working_on', 'Change_of_consistency', 'Execution', 'Success_or_failure', 'Work', 'Supply', 'Differentiation', 'Placing', 'Submitting_documents', 'Cooking_creation', 'Cause_to_start', 'Leadership', 'Successful_action', 'Building', 'Setting_out', 'Dressing', 'Verdict', 'Compliance', 'Posing_as', 'Arranging', 'Feigning', 'Categorization', 'Change_event_time', 'Causation', 'Cause_change_of_consistency']</t>
+  </si>
+  <si>
+    <t>['Process_end', 'Reasoning', 'Taking', 'Being_employed', 'Choosing', 'Working_on', 'Change_of_leadership', 'Killing', 'Activity_stop', 'Work', 'Coming_to_believe', 'Firing', 'Activity_finish', 'Notification_of_charges', 'Cause_to_end', 'Deciding', 'Contingency', 'Commerce_collect', 'Manipulation']</t>
+  </si>
+  <si>
+    <t>['Cause_motion', 'Leadership', 'Using', 'Operating_a_system', 'Sending', 'Being_in_operation', 'Influence_of_event_on_cognizer']</t>
+  </si>
+  <si>
+    <t>['Reporting', 'Evidence', 'Create_representation', 'Reasoning', 'Intentionally_create', 'Create_physical_artwork', 'Sign_agreement', 'Communicate_categorization', 'Ratification', 'Hiring', 'Adorning', 'Statement']</t>
+  </si>
+  <si>
+    <t>['Supply', 'Forgiveness', 'Assistance']</t>
+  </si>
+  <si>
+    <t>['Besieging', 'Locative_relation']</t>
+  </si>
+  <si>
+    <t>['Getting', 'Taking']</t>
+  </si>
+  <si>
+    <t>['Taking', 'Inchoative_attaching', 'Change_event_duration', 'Process_stop', 'Halt', 'Attaching', 'Being_in_operation', 'Cause_motion', 'Activity_stop', 'Becoming', 'Success_or_failure', 'Placing', 'Retaining', 'Resolve_problem', 'Change_position_on_a_scale', 'Leadership', 'Motion', 'Successful_action', 'Using', 'Cause_change_of_position_on_a_scale', 'Travel', 'Activity_ongoing', 'Self_motion', 'Compliance', 'Being_attached', 'Manipulation', 'Change_event_time', 'Operating_a_system', 'Process_continue', 'Defend', 'Containing']</t>
+  </si>
+  <si>
+    <t>['Taking', 'Intentionally_act', 'Change_of_leadership', 'Being_in_operation', 'Removing', 'Influence_of_event_on_cognizer', 'Intentionally_create', 'Success_or_failure', 'Resolve_problem', 'Leadership', 'Successful_action', 'Using', 'Cotheme', 'Cause_to_make_progress', 'Verdict', 'Self_motion', 'Operating_a_system', 'Bringing', 'Causation']</t>
+  </si>
+  <si>
+    <t>['Adopt_selection', 'Cause_motion', 'Imposing_obligation', 'Manipulation', 'Change_of_leadership', 'Objective_influence', 'Impact', 'Being_in_effect', 'Attempt_suasion', 'Cause_to_move_in_place', 'Containing']</t>
+  </si>
+  <si>
+    <t>['Imprisonment', 'Departing', 'Ingestion', 'Encoding', 'Change_of_consistency', 'Cause_motion', 'Execution', 'Placing', 'Cooking_creation', 'Cause_to_start', 'Possession', 'Building', 'Judgment', 'Setting_out', 'Dressing', 'Posing_as', 'Feigning', 'Change_event_time', 'Experiencer_focus', 'Causation', 'Cause_change_of_consistency']</t>
+  </si>
+  <si>
+    <t>['Leadership', 'Employing', 'Successful_action', 'Giving', 'Intentionally_affect', 'Using', 'Being_in_operation', 'Operating_a_system', 'Work', 'Success_or_failure', 'Assistance', 'Being_employed', 'Resolve_problem', 'Working_on', 'Using_resource', 'Self_motion']</t>
+  </si>
+  <si>
+    <t>['Communication_manner', 'Motion', 'Avoiding']</t>
+  </si>
+  <si>
+    <t>['Taking', 'Intentionally_act', 'Change_of_leadership', 'Being_in_operation', 'Removing', 'Influence_of_event_on_cognizer', 'Intentionally_create', 'Cause_motion', 'Success_or_failure', 'Resolve_problem', 'Leadership', 'Successful_action', 'Using', 'Cotheme', 'Cause_to_make_progress', 'Operate_vehicle', 'Verdict', 'Self_motion', 'Operating_a_system', 'Bringing', 'Causation']</t>
+  </si>
+  <si>
+    <t>['Awareness', 'Commitment', 'Respond_to_proposal', 'Receiving', 'Verification', 'Reveal_secret', 'Statement']</t>
+  </si>
+  <si>
+    <t>['Sentencing', 'Cause_motion', 'Verdict', 'Judgment_communication', 'Cause_harm']</t>
+  </si>
+  <si>
+    <t>['Quitting_a_place', 'Departing', 'Competition']</t>
+  </si>
+  <si>
+    <t>['Replacing', 'Compliance', 'Take_place_of', 'Relative_time']</t>
+  </si>
+  <si>
+    <t>['Giving', 'Avoiding', 'Placing', 'Discussion', 'Forgoing', 'Statement']</t>
+  </si>
+  <si>
+    <t>['Friction', 'Hostile_encounter', 'Moving_in_place', 'Undergo_change', 'Change_direction', 'Cause_to_move_in_place', 'Quarreling', 'Self_motion']</t>
+  </si>
+  <si>
+    <t>['Giving', 'Extradition', 'Motion']</t>
+  </si>
+  <si>
+    <t>['Reporting', 'Imposing_obligation', 'Request', 'Leadership', 'Motion', 'Filling', 'Dispersal', 'Speak_on_topic', 'Verdict', 'Telling', 'Statement']</t>
+  </si>
+  <si>
+    <t>{'Giving', 'Bringing', 'Transfer'}</t>
+  </si>
+  <si>
+    <t>{'Adjusting', 'Compliance', 'Successful_action', 'Success_or_failure', 'Choosing'}</t>
+  </si>
+  <si>
+    <t>{'Cause_to_end', 'Activity_stop', 'Deciding', 'Firing', 'Coming_to_believe', 'Activity_finish', 'Choosing', 'Killing'}</t>
+  </si>
+  <si>
+    <t>{'Using', 'Operating_a_system', 'Sending', 'Being_in_operation', 'Influence_of_event_on_cognizer'}</t>
+  </si>
+  <si>
+    <t>set()</t>
+  </si>
+  <si>
+    <t>{'Inchoative_attaching', 'Successful_action', 'Manipulation', 'Change_event_time', 'Success_or_failure', 'Activity_ongoing'}</t>
+  </si>
+  <si>
+    <t>{'Leadership', 'Taking', 'Bringing', 'Cotheme', 'Causation', 'Removing', 'Influence_of_event_on_cognizer'}</t>
   </si>
   <si>
     <t>{'Adopt_selection', 'Imposing_obligation', 'Attempt_suasion'}</t>
   </si>
   <si>
-    <t>{'Judgment', 'Experiencer_focus'}</t>
-  </si>
-  <si>
-    <t>{'Quarreling', 'Hostile_encounter'}</t>
-  </si>
-  <si>
-    <t>{'Being_in_operation', 'Assistance', 'Operating_a_system', 'Using', 'Intentionally_affect'}</t>
-  </si>
-  <si>
-    <t>set()</t>
+    <t>{'Experiencer_focus', 'Judgment'}</t>
+  </si>
+  <si>
+    <t>{'Hostile_encounter', 'Quarreling'}</t>
+  </si>
+  <si>
+    <t>{'Intentionally_affect', 'Using', 'Operating_a_system', 'Assistance', 'Being_in_operation'}</t>
   </si>
   <si>
     <t>{'Reveal_secret', 'Statement'}</t>
@@ -445,61 +553,82 @@
     <t>{'Judgment_communication', 'Sentencing'}</t>
   </si>
   <si>
+    <t>{'Relative_time'}</t>
+  </si>
+  <si>
     <t>{'Giving'}</t>
   </si>
   <si>
-    <t>{'Request', 'Imposing_obligation', 'Leadership'}</t>
-  </si>
-  <si>
-    <t>{'Surrendering', 'Giving', 'Transfer', 'Desiring', 'Cotheme', 'Bringing', 'Submitting_documents', 'Intentionally_act', 'Delivery', 'Causation', 'Successfully_communicate_message', 'Motion'}</t>
-  </si>
-  <si>
-    <t>{'Supply', 'Working_on', 'Execution', 'Causation', 'Categorization', 'Setting_out', 'Ingestion', 'Judgment', 'Posing_as', 'Departing', 'Being_employed', 'Separating', 'Bail_setting', 'Cooking_creation', 'Change_event_time', 'Adjusting', 'Leadership', 'Work', 'Cause_to_start', 'Imprisonment', 'Dressing', 'Placing', 'Assistance', 'Verdict', 'Change_of_consistency', 'Differentiation', 'Encoding', 'Building', 'Feigning', 'Cause_change_of_consistency', 'Successful_action', 'Arranging', 'Removing', 'Success_or_failure'}</t>
-  </si>
-  <si>
-    <t>{'Working_on', 'Activity_stop', 'Deciding', 'Cause_to_end', 'Contingency', 'Reasoning', 'Process_end', 'Taking', 'Coming_to_believe', 'Work', 'Activity_finish', 'Firing', 'Arrest', 'Being_employed', 'Change_of_leadership', 'Notification_of_charges', 'Choosing', 'Kidnapping', 'Commerce_collect', 'Manipulation', 'Killing'}</t>
-  </si>
-  <si>
-    <t>{'Statement', 'Inchoative_attaching', 'Hiring', 'Inhibit_movement', 'Activity_stop', 'Wearing', 'Being_in_operation', 'Becoming', 'Operating_a_system', 'Resolve_problem', 'Compliance', 'Process_continue', 'Taking', 'Leadership', 'Halt', 'Change_position_on_a_scale', 'Placing', 'Being_attached', 'Success_or_failure', 'Cause_motion', 'Motion', 'Retaining', 'Containing', 'Arrest', 'Attaching', 'Cause_change_of_position_on_a_scale', 'Travel', 'Self_motion', 'Change_event_time', 'Defend', 'Kidnapping', 'Manipulation', 'Change_event_duration', 'Process_stop', 'Using', 'Successful_action', 'Activity_ongoing', 'Detaining'}</t>
-  </si>
-  <si>
-    <t>{'Being_in_operation', 'Cause_to_make_progress', 'Resolve_problem', 'Operating_a_system', 'Taking', 'Leadership', 'Bringing', 'Verdict', 'Successful_action', 'Removing', 'Success_or_failure', 'Influence_of_event_on_cognizer', 'Self_motion', 'Change_of_leadership', 'Cotheme', 'Talking_into', 'Experiencer_obj', 'Intentionally_act', 'Intentionally_create', 'Using', 'Causation'}</t>
-  </si>
-  <si>
-    <t>{'Containing', 'Imposing_obligation', 'Attempt_suasion', 'Impact', 'Objective_influence', 'Adopt_selection', 'Manipulation', 'Cause_to_move_in_place', 'Change_of_leadership', 'Being_in_effect', 'Cause_motion'}</t>
-  </si>
-  <si>
-    <t>{'Execution', 'Causation', 'Setting_out', 'Ingestion', 'Posing_as', 'Judgment', 'Departing', 'Gathering_up', 'Cooking_creation', 'Possession', 'Change_event_time', 'Cause_to_start', 'Experiencer_focus', 'Imprisonment', 'Dressing', 'Placing', 'Change_of_consistency', 'Commerce_collect', 'Encoding', 'Building', 'Feigning', 'Cause_change_of_consistency', 'Come_together', 'Frugality', 'Removing', 'Cause_motion'}</t>
-  </si>
-  <si>
-    <t>{'Working_on', 'Filling', 'Being_in_operation', 'Giving', 'Using_resource', 'Resolve_problem', 'Operating_a_system', 'Rite', 'Leadership', 'Work', 'Employing', 'Intentionally_affect', 'Success_or_failure', 'Ingest_substance', 'Ingestion', 'Being_employed', 'Self_motion', 'Assistance', 'Using', 'Successful_action'}</t>
-  </si>
-  <si>
-    <t>{'Avoiding', 'Communication_manner', 'Motion'}</t>
-  </si>
-  <si>
-    <t>{'Being_in_operation', 'Cause_to_make_progress', 'Resolve_problem', 'Operating_a_system', 'Taking', 'Leadership', 'Bringing', 'Verdict', 'Successful_action', 'Removing', 'Success_or_failure', 'Operate_vehicle', 'Cause_motion', 'Sending', 'Contacting', 'Influence_of_event_on_cognizer', 'Self_motion', 'Change_of_leadership', 'Cotheme', 'Talking_into', 'Experiencer_obj', 'Intentionally_act', 'Intentionally_create', 'Using', 'Causation'}</t>
-  </si>
-  <si>
-    <t>{'Awareness', 'Statement', 'Verification', 'Commitment', 'Receiving', 'Reveal_secret', 'Respond_to_proposal'}</t>
-  </si>
-  <si>
-    <t>{'Judgment_communication', 'Verdict', 'Cause_harm', 'Sentencing', 'Cause_motion'}</t>
-  </si>
-  <si>
-    <t>{'Departing', 'Quitting_a_place', 'Competition'}</t>
-  </si>
-  <si>
-    <t>{'Supply', 'Giving', 'Assistance', 'Dispersal', 'Forgiveness'}</t>
-  </si>
-  <si>
-    <t>{'Friction', 'Jury_deliberation', 'Hostile_encounter', 'Undergo_change', 'Cause_to_move_in_place', 'Moving_in_place', 'Change_direction', 'Self_motion', 'Quarreling', 'Discussion'}</t>
-  </si>
-  <si>
-    <t>{'Extradition', 'Submitting_documents', 'Surrendering', 'Giving', 'Causation', 'Motion'}</t>
-  </si>
-  <si>
-    <t>{'Needing', 'Judgment_communication', 'Required_event', 'Telling', 'Reporting', 'Filling', 'Statement', 'Taking_time', 'Imposing_obligation', 'Judgment', 'Dispersal', 'Have_as_requirement', 'Verdict', 'Request', 'Omen', 'Speak_on_topic', 'Motion', 'Leadership'}</t>
+    <t>{'Imposing_obligation', 'Leadership', 'Request'}</t>
+  </si>
+  <si>
+    <t>{'Surrendering', 'Motion', 'Giving', 'Cotheme', 'Intentionally_act', 'Successfully_communicate_message', 'Bringing', 'Transfer', 'Delivery', 'Submitting_documents', 'Causation', 'Desiring'}</t>
+  </si>
+  <si>
+    <t>{'Adjusting', 'Imprisonment', 'Departing', 'Ingestion', 'Assistance', 'Being_employed', 'Encoding', 'Separating', 'Choosing', 'Working_on', 'Removing', 'Change_of_consistency', 'Execution', 'Success_or_failure', 'Work', 'Supply', 'Differentiation', 'Placing', 'Submitting_documents', 'Cooking_creation', 'Cause_to_start', 'Leadership', 'Successful_action', 'Judgment', 'Building', 'Setting_out', 'Dressing', 'Verdict', 'Compliance', 'Bail_setting', 'Posing_as', 'Arranging', 'Feigning', 'Categorization', 'Change_event_time', 'Causation', 'Cause_change_of_consistency'}</t>
+  </si>
+  <si>
+    <t>{'Process_end', 'Reasoning', 'Taking', 'Being_employed', 'Choosing', 'Working_on', 'Change_of_leadership', 'Killing', 'Activity_stop', 'Work', 'Firing', 'Coming_to_believe', 'Activity_finish', 'Notification_of_charges', 'Arrest', 'Kidnapping', 'Cause_to_end', 'Deciding', 'Contingency', 'Commerce_collect', 'Manipulation'}</t>
+  </si>
+  <si>
+    <t>{'Sending', 'Cause_motion', 'Leadership', 'Using', 'Being_in_operation', 'Operating_a_system', 'Influence_of_event_on_cognizer'}</t>
+  </si>
+  <si>
+    <t>{'Intentionally_create', 'Reporting', 'Evidence', 'Create_representation', 'Reasoning', 'Text_creation', 'Create_physical_artwork', 'Sign_agreement', 'Communicate_categorization', 'Ratification', 'Hiring', 'Adorning', 'Get_a_job', 'Statement'}</t>
+  </si>
+  <si>
+    <t>{'Giving', 'Forgiveness', 'Assistance', 'Supply', 'Dispersal'}</t>
+  </si>
+  <si>
+    <t>{'Besieging', 'Locative_relation'}</t>
+  </si>
+  <si>
+    <t>{'Getting', 'Taking'}</t>
+  </si>
+  <si>
+    <t>{'Inchoative_attaching', 'Taking', 'Change_event_duration', 'Process_stop', 'Halt', 'Attaching', 'Wearing', 'Being_in_operation', 'Cause_motion', 'Activity_stop', 'Becoming', 'Success_or_failure', 'Placing', 'Retaining', 'Resolve_problem', 'Arrest', 'Kidnapping', 'Change_position_on_a_scale', 'Leadership', 'Successful_action', 'Motion', 'Using', 'Cause_change_of_position_on_a_scale', 'Containing', 'Detaining', 'Travel', 'Activity_ongoing', 'Self_motion', 'Compliance', 'Inhibit_movement', 'Manipulation', 'Change_event_time', 'Being_attached', 'Operating_a_system', 'Hiring', 'Process_continue', 'Defend', 'Statement'}</t>
+  </si>
+  <si>
+    <t>{'Taking', 'Talking_into', 'Experiencer_obj', 'Intentionally_act', 'Change_of_leadership', 'Being_in_operation', 'Removing', 'Influence_of_event_on_cognizer', 'Intentionally_create', 'Success_or_failure', 'Resolve_problem', 'Leadership', 'Successful_action', 'Using', 'Cotheme', 'Cause_to_make_progress', 'Verdict', 'Self_motion', 'Operating_a_system', 'Bringing', 'Causation'}</t>
+  </si>
+  <si>
+    <t>{'Adopt_selection', 'Imposing_obligation', 'Cause_motion', 'Manipulation', 'Change_of_leadership', 'Objective_influence', 'Impact', 'Being_in_effect', 'Attempt_suasion', 'Cause_to_move_in_place', 'Containing'}</t>
+  </si>
+  <si>
+    <t>{'Imprisonment', 'Cause_to_start', 'Departing', 'Possession', 'Ingestion', 'Judgment', 'Building', 'Commerce_collect', 'Setting_out', 'Encoding', 'Dressing', 'Removing', 'Change_of_consistency', 'Cause_motion', 'Posing_as', 'Execution', 'Feigning', 'Change_event_time', 'Experiencer_focus', 'Come_together', 'Frugality', 'Placing', 'Gathering_up', 'Causation', 'Cause_change_of_consistency', 'Cooking_creation'}</t>
+  </si>
+  <si>
+    <t>{'Giving', 'Ingestion', 'Assistance', 'Being_employed', 'Working_on', 'Being_in_operation', 'Rite', 'Employing', 'Intentionally_affect', 'Success_or_failure', 'Work', 'Resolve_problem', 'Ingest_substance', 'Leadership', 'Successful_action', 'Using', 'Self_motion', 'Operating_a_system', 'Filling', 'Using_resource'}</t>
+  </si>
+  <si>
+    <t>{'Communication_manner', 'Motion', 'Avoiding'}</t>
+  </si>
+  <si>
+    <t>{'Taking', 'Talking_into', 'Experiencer_obj', 'Sending', 'Intentionally_act', 'Change_of_leadership', 'Being_in_operation', 'Removing', 'Influence_of_event_on_cognizer', 'Intentionally_create', 'Cause_motion', 'Success_or_failure', 'Resolve_problem', 'Leadership', 'Successful_action', 'Using', 'Cotheme', 'Cause_to_make_progress', 'Operate_vehicle', 'Verdict', 'Self_motion', 'Contacting', 'Operating_a_system', 'Bringing', 'Causation'}</t>
+  </si>
+  <si>
+    <t>{'Commitment', 'Awareness', 'Respond_to_proposal', 'Receiving', 'Verification', 'Reveal_secret', 'Statement'}</t>
+  </si>
+  <si>
+    <t>{'Sentencing', 'Cause_motion', 'Cause_harm', 'Judgment_communication', 'Verdict'}</t>
+  </si>
+  <si>
+    <t>{'Competition', 'Quitting_a_place', 'Departing'}</t>
+  </si>
+  <si>
+    <t>{'Compliance', 'Successful_action', 'Success_or_failure', 'Take_place_of', 'Relative_time', 'Replacing'}</t>
+  </si>
+  <si>
+    <t>{'Grant_permission', 'Giving', 'Permitting', 'Avoiding', 'Placing', 'Discussion', 'Forgoing', 'Statement'}</t>
+  </si>
+  <si>
+    <t>{'Friction', 'Hostile_encounter', 'Jury_deliberation', 'Moving_in_place', 'Discussion', 'Undergo_change', 'Change_direction', 'Cause_to_move_in_place', 'Quarreling', 'Self_motion'}</t>
+  </si>
+  <si>
+    <t>{'Surrendering', 'Motion', 'Giving', 'Submitting_documents', 'Causation', 'Extradition'}</t>
+  </si>
+  <si>
+    <t>{'Imposing_obligation', 'Judgment_communication', 'Omen', 'Needing', 'Dispersal', 'Reporting', 'Leadership', 'Motion', 'Judgment', 'Taking_time', 'Verdict', 'Prohibiting', 'Deny_permission', 'Request', 'Have_as_requirement', 'Filling', 'Required_event', 'Preventing', 'Speak_on_topic', 'Telling', 'Statement'}</t>
   </si>
 </sst>
 </file>
@@ -857,7 +986,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -912,28 +1041,28 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="L2" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -947,28 +1076,28 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="K3" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="L3" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -982,208 +1111,208 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="K4" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="L4" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5">
-        <v>1430</v>
+        <v>1074</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="J5" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="K5" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="L5" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6">
-        <v>1444</v>
+        <v>1111</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="J6" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="K6" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="L6" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7">
-        <v>1453</v>
+        <v>1118</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>99</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="J7" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="L7" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>1457</v>
+        <v>1174</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="J8" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="L8" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>1458</v>
+        <v>1226</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="J9" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="K9" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="L9" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10">
-        <v>1459</v>
+        <v>1430</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1192,208 +1321,208 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="I10" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="K10" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="L10" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11">
-        <v>1537</v>
+        <v>1444</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="J11" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="K11" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="L11" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12">
-        <v>1552</v>
+        <v>1453</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="J12" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="K12" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="L12" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>1582</v>
+        <v>1457</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="J13" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="K13" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="L13" t="s">
-        <v>154</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>1596</v>
+        <v>1458</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="J14" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="K14" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="L14" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>1600</v>
+        <v>1459</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="I15" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="J15" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="K15" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="L15" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>1634</v>
+        <v>1537</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1402,33 +1531,33 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>111</v>
       </c>
       <c r="I16" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="J16" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="K16" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17">
-        <v>1646</v>
+        <v>1552</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
@@ -1437,33 +1566,33 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="I17" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="K17" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="L17" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>1697</v>
+        <v>1582</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -1472,33 +1601,33 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="J18" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="K18" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="L18" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
-        <v>1722</v>
+        <v>1596</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -1507,33 +1636,33 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="J19" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="K19" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="L19" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20">
-        <v>1723</v>
+        <v>1600</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
@@ -1542,33 +1671,33 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="I20" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="K20" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="L20" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21">
-        <v>1725</v>
+        <v>1634</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
@@ -1577,33 +1706,33 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" t="s">
-        <v>79</v>
+        <v>91</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="K21" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="L21" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22">
-        <v>1726</v>
+        <v>1646</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -1612,33 +1741,33 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" t="s">
-        <v>79</v>
+        <v>92</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="I22" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K22" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="L22" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23">
-        <v>1729</v>
+        <v>1661</v>
       </c>
       <c r="B23" t="s">
         <v>33</v>
@@ -1647,33 +1776,33 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="G23" t="s">
+        <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="J23" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="K23" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="L23" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24">
-        <v>1751</v>
+        <v>1697</v>
       </c>
       <c r="B24" t="s">
         <v>34</v>
@@ -1682,28 +1811,273 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
       </c>
       <c r="H24" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" t="s">
+        <v>148</v>
+      </c>
+      <c r="K24" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>1719</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" t="s">
+        <v>162</v>
+      </c>
+      <c r="K25" t="s">
+        <v>170</v>
+      </c>
+      <c r="L25" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>1722</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" t="s">
+        <v>163</v>
+      </c>
+      <c r="K26" t="s">
+        <v>175</v>
+      </c>
+      <c r="L26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>1723</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" t="s">
         <v>96</v>
       </c>
-      <c r="I24" t="s">
-        <v>106</v>
-      </c>
-      <c r="J24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" t="s">
-        <v>140</v>
-      </c>
-      <c r="L24" t="s">
-        <v>140</v>
+      <c r="G27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" t="s">
+        <v>164</v>
+      </c>
+      <c r="K27" t="s">
+        <v>180</v>
+      </c>
+      <c r="L27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>1725</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" t="s">
+        <v>164</v>
+      </c>
+      <c r="K28" t="s">
+        <v>180</v>
+      </c>
+      <c r="L28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>1726</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" t="s">
+        <v>141</v>
+      </c>
+      <c r="J29" t="s">
+        <v>164</v>
+      </c>
+      <c r="K29" t="s">
+        <v>180</v>
+      </c>
+      <c r="L29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>1729</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" t="s">
+        <v>142</v>
+      </c>
+      <c r="J30" t="s">
+        <v>165</v>
+      </c>
+      <c r="K30" t="s">
+        <v>181</v>
+      </c>
+      <c r="L30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>1751</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>121</v>
+      </c>
+      <c r="I31" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" t="s">
+        <v>128</v>
+      </c>
+      <c r="K31" t="s">
+        <v>170</v>
+      </c>
+      <c r="L31" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>